<commit_message>
adding correct headers to rate_birth and life expectancy
</commit_message>
<xml_diff>
--- a/autumn/xls/life_expectancy_2014.xlsx
+++ b/autumn/xls/life_expectancy_2014.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\swas0001\unc_storage_AuTuMN\autumn\xls\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="480" yWindow="60" windowWidth="18075" windowHeight="9900"/>
   </bookViews>
@@ -16,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2167" uniqueCount="744">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2167" uniqueCount="745">
   <si>
     <t>Iraq</t>
   </si>
@@ -2248,12 +2253,15 @@
   </si>
   <si>
     <t>Cameroon</t>
+  </si>
+  <si>
+    <t>country</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -2295,6 +2303,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -2343,7 +2354,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2378,7 +2389,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2589,7 +2600,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BH252"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2619,7 +2632,7 @@
     </row>
     <row r="4" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>722</v>
+        <v>744</v>
       </c>
       <c r="B4" t="s">
         <v>486</v>

</xml_diff>